<commit_message>
Import LIB_BRANCHE_OPTION when importing student file
</commit_message>
<xml_diff>
--- a/stages/test_files/EXPORT_GAN.xlsx
+++ b/stages/test_files/EXPORT_GAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t xml:space="preserve">NOCLOEE</t>
   </si>
@@ -91,6 +91,9 @@
     <t xml:space="preserve">CODE_BRANCH_OPTION</t>
   </si>
   <si>
+    <t xml:space="preserve">LIB_BRANCHE_OPTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANNEE_EN_COURS</t>
   </si>
   <si>
@@ -184,6 +187,9 @@
     <t xml:space="preserve">ENF</t>
   </si>
   <si>
+    <t xml:space="preserve">Accompagnement des enfants</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crèche Les Mousaillons</t>
   </si>
   <si>
@@ -236,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">1EDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boulanger (à ignorer)</t>
   </si>
 </sst>
 </file>
@@ -360,19 +369,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="1" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="35" min="22" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="43.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="37" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="36" min="22" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="43.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,109 +499,115 @@
       <c r="AL1" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>164718</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="X2" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="0" t="n">
         <v>20162017</v>
       </c>
-      <c r="Y2" s="3" t="n">
+      <c r="Z2" s="3" t="n">
         <v>42597</v>
       </c>
-      <c r="Z2" s="3" t="n">
+      <c r="AA2" s="3" t="n">
         <v>43691</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AB2" s="0" t="n">
         <v>44444</v>
       </c>
-      <c r="AB2" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="AC2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF2" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="0" t="n">
         <v>22222</v>
       </c>
-      <c r="AG2" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="AH2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AJ2" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="AK2" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="AL2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>10</v>
       </c>
@@ -600,43 +615,46 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>23208</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK3" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed student import when birth_date or option_ase are empty
</commit_message>
<xml_diff>
--- a/stages/test_files/EXPORT_GAN.xlsx
+++ b/stages/test_files/EXPORT_GAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t xml:space="preserve">NOCLOEE</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">Boulanger (à ignorer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irène</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -657,6 +660,51 @@
         <v>64</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>